<commit_message>
Add scheduling files and update course data
Added Daftar_Mata_Kuliah_Lengkap.csv, jadwal_terbaik.csv, and penjadwalan_ga.html for course and schedule management. Updated Daftar_Mata_Kuliah_Lengkap.xlsx and penjadwalan_ga.ipynb, and removed Daftar_matkul.csv to consolidate course data sources.
</commit_message>
<xml_diff>
--- a/Daftar_Mata_Kuliah_Lengkap.xlsx
+++ b/Daftar_Mata_Kuliah_Lengkap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rioad\Documents\Kuliah\Semester 7\Algoritma Genetika\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c57fd381dd02afd/Dokumen/GitHub/Ag/Penjadwalan_algoritma_genetika/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A6D0A6-59E5-49D5-BE93-1E75F4249923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{00A6D0A6-59E5-49D5-BE93-1E75F4249923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{263FEF1E-3666-4B43-96A3-DBBA01AADD04}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="100">
-  <si>
-    <t>Semester</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="99">
   <si>
     <t>Agama Kristen Protestan</t>
   </si>
@@ -202,9 +199,6 @@
     <t>Drs. Sartana., M.Si</t>
   </si>
   <si>
-    <t>Daftar Mata Kuliah Semester Ganjil 2025/2026</t>
-  </si>
-  <si>
     <t>MKI112206</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
     <t>kelas</t>
   </si>
   <si>
-    <t>jenis_dosen</t>
-  </si>
-  <si>
     <t>DLB</t>
   </si>
   <si>
@@ -320,6 +311,12 @@
   </si>
   <si>
     <t>DOSEN TETAP</t>
+  </si>
+  <si>
+    <t>tipe_dosen</t>
+  </si>
+  <si>
+    <t>semester</t>
   </si>
 </sst>
 </file>
@@ -666,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -708,15 +705,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -745,6 +733,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,6 +754,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1049,926 +1047,918 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L33"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.90625" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" customWidth="1"/>
+    <col min="5" max="5" width="46.453125" customWidth="1"/>
+    <col min="6" max="6" width="7.90625" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="21" t="s">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="29">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="17" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="19" t="s">
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="29">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="29">
+        <v>1</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="32">
-        <v>1</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="29">
+        <v>1</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="22"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="32">
-        <v>1</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2</v>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>97</v>
+        <v>51</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="J6" s="5">
         <v>2</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="22"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="32">
-        <v>1</v>
-      </c>
-      <c r="C7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="29">
+        <v>1</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
         <v>2</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>96</v>
+        <v>52</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J7" s="5">
         <v>3</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="32">
-        <v>1</v>
-      </c>
-      <c r="C8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="29">
+        <v>1</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
         <v>2</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>96</v>
+        <v>52</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J8" s="5">
         <v>4</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="32">
-        <v>1</v>
-      </c>
-      <c r="C9" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="29">
+        <v>1</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2</v>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>97</v>
+      <c r="G9" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="J9" s="5">
         <v>5</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="32">
-        <v>1</v>
-      </c>
-      <c r="C10" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="33"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
+        <v>1</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2</v>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>97</v>
+      <c r="G10" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="J10" s="5">
         <v>6</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="22"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="32">
-        <v>1</v>
-      </c>
-      <c r="C11" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="33"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
+        <v>1</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1">
-        <v>3</v>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>96</v>
+        <v>52</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="32">
-        <v>1</v>
-      </c>
-      <c r="C12" s="25" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
+        <v>1</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>96</v>
+        <v>52</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="32">
-        <v>1</v>
-      </c>
-      <c r="C13" s="25" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="29">
+        <v>1</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1">
         <v>2</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="J13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="K13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="32">
-        <v>1</v>
-      </c>
-      <c r="C14" s="25" t="s">
+      <c r="L13" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="30">
+        <v>1</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
         <v>2</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J14" s="5">
         <v>1</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="23"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="32">
-        <v>1</v>
-      </c>
-      <c r="C15" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" s="34"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="26">
+        <v>1</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="C15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="8">
         <v>2</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>96</v>
+      <c r="E15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J15" s="5">
         <v>2</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="23"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="33">
-        <v>1</v>
-      </c>
-      <c r="C16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="34"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="32">
+        <v>3</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2">
         <v>2</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>97</v>
+      <c r="E16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="J16" s="5">
         <v>3</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="23"/>
-    </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29">
-        <v>1</v>
-      </c>
-      <c r="C17" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="34"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="29">
+        <v>3</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="8">
-        <v>2</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>97</v>
+      <c r="F17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J17" s="5">
         <v>4</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="35">
-        <v>3</v>
-      </c>
-      <c r="C18" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="34"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="29">
+        <v>3</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>97</v>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J18" s="5">
         <v>5</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="32">
-        <v>3</v>
-      </c>
-      <c r="C19" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="34"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="29">
+        <v>3</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J19" s="5">
         <v>6</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L19" s="23"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="32">
-        <v>3</v>
-      </c>
-      <c r="C20" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="34"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="29">
+        <v>3</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3</v>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J20" s="5">
         <v>7</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="23"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="32">
-        <v>3</v>
-      </c>
-      <c r="C21" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="34"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="29">
+        <v>3</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2</v>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J21" s="5">
         <v>8</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L21" s="23"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="32">
-        <v>3</v>
-      </c>
-      <c r="C22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="34"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="29">
+        <v>3</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2</v>
+      <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J22" s="5">
         <v>9</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L22" s="23"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="32">
-        <v>3</v>
-      </c>
-      <c r="C23" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="34"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="29">
+        <v>3</v>
+      </c>
+      <c r="B23" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="1">
-        <v>3</v>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J23" s="5">
         <v>10</v>
       </c>
       <c r="K23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L23" s="34"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="29">
+        <v>3</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="32">
-        <v>3</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J24" s="5">
         <v>11</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L24" s="23"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="32">
-        <v>3</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="1">
-        <v>3</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>97</v>
+        <v>46</v>
+      </c>
+      <c r="L24" s="34"/>
+    </row>
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="31">
+        <v>3</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="8">
+        <v>2</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="J25" s="5">
         <v>12</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L25" s="23"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="32">
-        <v>3</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>97</v>
+      <c r="L25" s="34"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="32">
+        <v>5</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J26" s="5">
         <v>13</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L26" s="23"/>
-    </row>
-    <row r="27" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="34">
-        <v>3</v>
-      </c>
-      <c r="C27" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="L26" s="34"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="29">
+        <v>5</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="8">
-        <v>2</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>97</v>
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J27" s="5">
         <v>14</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L27" s="23"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="35">
+        <v>49</v>
+      </c>
+      <c r="L27" s="34"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="29">
         <v>5</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="B28" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="2">
-        <v>3</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>97</v>
+      <c r="C28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J28" s="5">
         <v>15</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L28" s="23"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="32">
+        <v>50</v>
+      </c>
+      <c r="L28" s="34"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="29">
         <v>5</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="1">
-        <v>3</v>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J29" s="5">
         <v>16</v>
       </c>
       <c r="K29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L29" s="34"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="31">
+        <v>5</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="8">
+        <v>3</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L29" s="23"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="32">
-        <v>5</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="32">
-        <v>5</v>
-      </c>
-      <c r="C31" s="25" t="s">
+      <c r="F30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="28">
+        <v>7</v>
+      </c>
+      <c r="B31" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="1">
-        <v>3</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="34">
-        <v>5</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" s="8" t="s">
+      <c r="C31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="8">
-        <v>3</v>
-      </c>
-      <c r="F32" s="8" t="s">
+      <c r="D31" s="4">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="31">
-        <v>7</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="4">
-        <v>3</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>97</v>
+      <c r="F31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D2:F2"/>
+  <mergeCells count="2">
     <mergeCell ref="L4:L10"/>
     <mergeCell ref="L13:L29"/>
   </mergeCells>

</xml_diff>